<commit_message>
[md] edit README file
</commit_message>
<xml_diff>
--- a/TableDefaultColumns.xlsx
+++ b/TableDefaultColumns.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\yoo\개발관련\BDC\데이터 품질 체크기\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\yoo\개발관련\BDC\Digital-Industry-Innovation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C3A2A5-1786-49DB-B8ED-F1119823950C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C63A9FE-83A4-4319-A8EB-C10622AC7CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="재무_columnsl" sheetId="1" r:id="rId1"/>
-    <sheet name="일반_columns" sheetId="3" r:id="rId2"/>
-    <sheet name="table" sheetId="2" r:id="rId3"/>
+    <sheet name="한국_columns" sheetId="4" r:id="rId1"/>
+    <sheet name="재무_columns" sheetId="1" r:id="rId2"/>
+    <sheet name="일반_columns" sheetId="3" r:id="rId3"/>
+    <sheet name="table" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="373">
   <si>
     <t>표준_영문컬럼명</t>
   </si>
@@ -1237,13 +1237,19 @@
   <si>
     <t>VARCHAR(8)</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>법인등록번호</t>
+  </si>
+  <si>
+    <t>사업자등록번호</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1315,6 +1321,12 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1354,7 +1366,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1370,6 +1382,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1651,11 +1668,771 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4ECE1D-62E8-4122-8E8B-195D2D8071EB}">
+  <dimension ref="A1:C82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="8"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="8"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="8"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="8"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="8"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="8"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="8"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="8"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="8"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="8"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="8"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="8"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="8"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" s="8"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="8"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="8"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" s="8"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="8"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" s="8"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" s="8"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="8"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C65" s="8"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66" s="8"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="8"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" s="8"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69" s="8"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="8"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C71" s="8"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72" s="8"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C73" s="8"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" s="8"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C75" s="8"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="8"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C77" s="8"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C78" s="8"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C79" s="8"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" s="8"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C81" s="8"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C82" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2574,7 +3351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D686ED2-ECA7-49CC-95F7-CBF3DE6ABFBD}">
   <dimension ref="A1:C59"/>
   <sheetViews>
@@ -3244,7 +4021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C28F45E-F065-4701-9A53-345D3CBE4263}">
   <dimension ref="A1:B42"/>
   <sheetViews>

</xml_diff>

<commit_message>
[py] add historical_data option and investing update
</commit_message>
<xml_diff>
--- a/TableDefaultColumns.xlsx
+++ b/TableDefaultColumns.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\yoo\개발관련\BDC\데이터 품질 체크기\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\yoo\개발관련\BDC\Digital-Industry-Innovation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C3A2A5-1786-49DB-B8ED-F1119823950C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C63A9FE-83A4-4319-A8EB-C10622AC7CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="재무_columnsl" sheetId="1" r:id="rId1"/>
-    <sheet name="일반_columns" sheetId="3" r:id="rId2"/>
-    <sheet name="table" sheetId="2" r:id="rId3"/>
+    <sheet name="한국_columns" sheetId="4" r:id="rId1"/>
+    <sheet name="재무_columns" sheetId="1" r:id="rId2"/>
+    <sheet name="일반_columns" sheetId="3" r:id="rId3"/>
+    <sheet name="table" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="373">
   <si>
     <t>표준_영문컬럼명</t>
   </si>
@@ -1237,13 +1237,19 @@
   <si>
     <t>VARCHAR(8)</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>법인등록번호</t>
+  </si>
+  <si>
+    <t>사업자등록번호</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1315,6 +1321,12 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1354,7 +1366,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1370,6 +1382,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1651,11 +1668,771 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4ECE1D-62E8-4122-8E8B-195D2D8071EB}">
+  <dimension ref="A1:C82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="8"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="8"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="8"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="8"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="8"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="8"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="8"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="8"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="8"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="8"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="8"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="8"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="8"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" s="8"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="8"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="8"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" s="8"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="8"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" s="8"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" s="8"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="8"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C65" s="8"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66" s="8"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="8"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" s="8"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69" s="8"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="8"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C71" s="8"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72" s="8"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C73" s="8"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" s="8"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C75" s="8"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="8"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C77" s="8"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C78" s="8"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C79" s="8"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" s="8"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C81" s="8"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C82" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2574,7 +3351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D686ED2-ECA7-49CC-95F7-CBF3DE6ABFBD}">
   <dimension ref="A1:C59"/>
   <sheetViews>
@@ -3244,7 +4021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C28F45E-F065-4701-9A53-345D3CBE4263}">
   <dimension ref="A1:B42"/>
   <sheetViews>

</xml_diff>